<commit_message>
updates made to application_data_condensed_df
</commit_message>
<xml_diff>
--- a/application_data_condensed_businessman_applicants_df.xlsx
+++ b/application_data_condensed_businessman_applicants_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="51">
   <si>
     <t>SK_ID_CURR</t>
   </si>
@@ -85,6 +85,9 @@
     <t>ORGANIZATION_TYPE</t>
   </si>
   <si>
+    <t>WEEKEND_APPR_PROCESS_START</t>
+  </si>
+  <si>
     <t>FRAUD_RISK</t>
   </si>
   <si>
@@ -139,25 +142,28 @@
     <t>FRIDAY</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>THURSDAY</t>
+  </si>
+  <si>
+    <t>TUESDAY</t>
+  </si>
+  <si>
+    <t>Self-employed</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Business Entity Type 3</t>
+  </si>
+  <si>
     <t>SATURDAY</t>
   </si>
   <si>
     <t>SUNDAY</t>
-  </si>
-  <si>
-    <t>THURSDAY</t>
-  </si>
-  <si>
-    <t>TUESDAY</t>
-  </si>
-  <si>
-    <t>Self-employed</t>
-  </si>
-  <si>
-    <t>Bank</t>
-  </si>
-  <si>
-    <t>Business Entity Type 3</t>
   </si>
   <si>
     <t>Low Risk</t>
@@ -518,13 +524,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,22 +603,25 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:25">
       <c r="A2">
         <v>134442</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -630,25 +639,25 @@
         <v>2250000</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R2">
         <v>2</v>
@@ -660,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="U2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V2">
         <v>14</v>
@@ -669,24 +678,27 @@
         <v>45</v>
       </c>
       <c r="X2" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:25">
       <c r="A3">
         <v>134526</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -704,22 +716,22 @@
         <v>1350000</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R3">
         <v>2</v>
@@ -731,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V3">
         <v>17</v>
@@ -740,24 +752,27 @@
         <v>46</v>
       </c>
       <c r="X3" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:25">
       <c r="A4">
         <v>201088</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -775,25 +790,25 @@
         <v>675000</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P4">
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R4">
         <v>3</v>
@@ -805,7 +820,7 @@
         <v>2</v>
       </c>
       <c r="U4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V4">
         <v>10</v>
@@ -816,22 +831,25 @@
       <c r="X4" t="s">
         <v>48</v>
       </c>
+      <c r="Y4" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:25">
       <c r="A5">
         <v>207018</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -849,25 +867,25 @@
         <v>540000</v>
       </c>
       <c r="K5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P5">
         <v>6</v>
       </c>
       <c r="Q5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R5">
         <v>1</v>
@@ -888,24 +906,27 @@
         <v>45</v>
       </c>
       <c r="X5" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:25">
       <c r="A6">
         <v>254395</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -923,25 +944,25 @@
         <v>1350000</v>
       </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P6">
         <v>8</v>
       </c>
       <c r="Q6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R6">
         <v>2</v>
@@ -962,24 +983,27 @@
         <v>45</v>
       </c>
       <c r="X6" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:25">
       <c r="A7">
         <v>268946</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -997,25 +1021,25 @@
         <v>2250000</v>
       </c>
       <c r="K7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P7">
         <v>5</v>
       </c>
       <c r="Q7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R7">
         <v>2</v>
@@ -1027,7 +1051,7 @@
         <v>2</v>
       </c>
       <c r="U7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V7">
         <v>16</v>
@@ -1036,24 +1060,27 @@
         <v>45</v>
       </c>
       <c r="X7" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:25">
       <c r="A8">
         <v>347590</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1071,25 +1098,25 @@
         <v>2250000</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P8">
         <v>4</v>
       </c>
       <c r="Q8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R8">
         <v>1</v>
@@ -1110,24 +1137,27 @@
         <v>45</v>
       </c>
       <c r="X8" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:25">
       <c r="A9">
         <v>372723</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1145,19 +1175,19 @@
         <v>900000</v>
       </c>
       <c r="K9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P9">
         <v>1</v>
@@ -1181,24 +1211,27 @@
         <v>47</v>
       </c>
       <c r="X9" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:25">
       <c r="A10">
         <v>394662</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1216,19 +1249,19 @@
         <v>225000</v>
       </c>
       <c r="K10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P10">
         <v>1</v>
@@ -1243,7 +1276,7 @@
         <v>3</v>
       </c>
       <c r="U10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V10">
         <v>16</v>
@@ -1252,24 +1285,27 @@
         <v>45</v>
       </c>
       <c r="X10" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:25">
       <c r="A11">
         <v>438579</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1287,22 +1323,22 @@
         <v>495000</v>
       </c>
       <c r="K11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R11">
         <v>2</v>
@@ -1314,7 +1350,7 @@
         <v>2</v>
       </c>
       <c r="U11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V11">
         <v>11</v>
@@ -1324,6 +1360,9 @@
       </c>
       <c r="X11" t="s">
         <v>48</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
conversation of HOUR_APPR_PROCESS_START values as strings and concated ':00:00' to create a time format
</commit_message>
<xml_diff>
--- a/application_data_condensed_businessman_applicants_df.xlsx
+++ b/application_data_condensed_businessman_applicants_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="58">
   <si>
     <t>SK_ID_CURR</t>
   </si>
@@ -149,6 +149,27 @@
   </si>
   <si>
     <t>TUESDAY</t>
+  </si>
+  <si>
+    <t>14:00:00</t>
+  </si>
+  <si>
+    <t>17:00:00</t>
+  </si>
+  <si>
+    <t>10:00:00</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
+    <t>11:00:00</t>
   </si>
   <si>
     <t>Self-employed</t>
@@ -671,17 +692,17 @@
       <c r="U2" t="s">
         <v>40</v>
       </c>
-      <c r="V2">
-        <v>14</v>
+      <c r="V2" t="s">
+        <v>45</v>
       </c>
       <c r="W2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="X2" t="s">
         <v>42</v>
       </c>
       <c r="Y2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -745,17 +766,17 @@
       <c r="U3" t="s">
         <v>41</v>
       </c>
-      <c r="V3">
-        <v>17</v>
+      <c r="V3" t="s">
+        <v>46</v>
       </c>
       <c r="W3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="X3" t="s">
         <v>42</v>
       </c>
       <c r="Y3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -822,17 +843,17 @@
       <c r="U4" t="s">
         <v>42</v>
       </c>
-      <c r="V4">
-        <v>10</v>
+      <c r="V4" t="s">
+        <v>47</v>
       </c>
       <c r="W4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="X4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="Y4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -899,17 +920,17 @@
       <c r="U5" t="s">
         <v>42</v>
       </c>
-      <c r="V5">
-        <v>14</v>
+      <c r="V5" t="s">
+        <v>45</v>
       </c>
       <c r="W5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="X5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="Y5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -976,17 +997,17 @@
       <c r="U6" t="s">
         <v>43</v>
       </c>
-      <c r="V6">
-        <v>15</v>
+      <c r="V6" t="s">
+        <v>48</v>
       </c>
       <c r="W6" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="X6" t="s">
         <v>42</v>
       </c>
       <c r="Y6" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1053,17 +1074,17 @@
       <c r="U7" t="s">
         <v>40</v>
       </c>
-      <c r="V7">
-        <v>16</v>
+      <c r="V7" t="s">
+        <v>49</v>
       </c>
       <c r="W7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="X7" t="s">
         <v>42</v>
       </c>
       <c r="Y7" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1130,17 +1151,17 @@
       <c r="U8" t="s">
         <v>44</v>
       </c>
-      <c r="V8">
-        <v>13</v>
+      <c r="V8" t="s">
+        <v>50</v>
       </c>
       <c r="W8" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="X8" t="s">
         <v>42</v>
       </c>
       <c r="Y8" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1204,17 +1225,17 @@
       <c r="U9" t="s">
         <v>44</v>
       </c>
-      <c r="V9">
-        <v>17</v>
+      <c r="V9" t="s">
+        <v>46</v>
       </c>
       <c r="W9" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="X9" t="s">
         <v>42</v>
       </c>
       <c r="Y9" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1278,17 +1299,17 @@
       <c r="U10" t="s">
         <v>40</v>
       </c>
-      <c r="V10">
-        <v>16</v>
+      <c r="V10" t="s">
+        <v>49</v>
       </c>
       <c r="W10" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="X10" t="s">
         <v>42</v>
       </c>
       <c r="Y10" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1352,17 +1373,17 @@
       <c r="U11" t="s">
         <v>42</v>
       </c>
-      <c r="V11">
-        <v>11</v>
+      <c r="V11" t="s">
+        <v>51</v>
       </c>
       <c r="W11" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="X11" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="Y11" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>